<commit_message>
Tabela de vendedores arrumada
</commit_message>
<xml_diff>
--- a/backend/uploads_app/resultado.xlsx
+++ b/backend/uploads_app/resultado.xlsx
@@ -34159,7 +34159,7 @@
         </is>
       </c>
       <c r="D508" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O508" t="inlineStr">
         <is>
@@ -34184,7 +34184,7 @@
         </is>
       </c>
       <c r="D509" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O509" t="inlineStr">
         <is>
@@ -34209,7 +34209,7 @@
         </is>
       </c>
       <c r="D510" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O510" t="inlineStr">
         <is>
@@ -34234,7 +34234,7 @@
         </is>
       </c>
       <c r="D511" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O511" t="inlineStr">
         <is>
@@ -34259,7 +34259,7 @@
         </is>
       </c>
       <c r="D512" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O512" t="inlineStr">
         <is>
@@ -34284,7 +34284,7 @@
         </is>
       </c>
       <c r="D513" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O513" t="inlineStr">
         <is>
@@ -34309,7 +34309,7 @@
         </is>
       </c>
       <c r="D514" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O514" t="inlineStr">
         <is>
@@ -34334,7 +34334,7 @@
         </is>
       </c>
       <c r="D515" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O515" t="inlineStr">
         <is>
@@ -34359,7 +34359,7 @@
         </is>
       </c>
       <c r="D516" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O516" t="inlineStr">
         <is>
@@ -34384,7 +34384,7 @@
         </is>
       </c>
       <c r="D517" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O517" t="inlineStr">
         <is>
@@ -34409,7 +34409,7 @@
         </is>
       </c>
       <c r="D518" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O518" t="inlineStr">
         <is>
@@ -34434,7 +34434,7 @@
         </is>
       </c>
       <c r="D519" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O519" t="inlineStr">
         <is>
@@ -34459,7 +34459,7 @@
         </is>
       </c>
       <c r="D520" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O520" t="inlineStr">
         <is>
@@ -34484,7 +34484,7 @@
         </is>
       </c>
       <c r="D521" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O521" t="inlineStr">
         <is>
@@ -34509,7 +34509,7 @@
         </is>
       </c>
       <c r="D522" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O522" t="inlineStr">
         <is>
@@ -34534,7 +34534,7 @@
         </is>
       </c>
       <c r="D523" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O523" t="inlineStr">
         <is>
@@ -34559,7 +34559,7 @@
         </is>
       </c>
       <c r="D524" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O524" t="inlineStr">
         <is>
@@ -34584,7 +34584,7 @@
         </is>
       </c>
       <c r="D525" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O525" t="inlineStr">
         <is>
@@ -34609,7 +34609,7 @@
         </is>
       </c>
       <c r="D526" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O526" t="inlineStr">
         <is>
@@ -34634,7 +34634,7 @@
         </is>
       </c>
       <c r="D527" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O527" t="inlineStr">
         <is>
@@ -34659,7 +34659,7 @@
         </is>
       </c>
       <c r="D528" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O528" t="inlineStr">
         <is>
@@ -34684,7 +34684,7 @@
         </is>
       </c>
       <c r="D529" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O529" t="inlineStr">
         <is>
@@ -34709,7 +34709,7 @@
         </is>
       </c>
       <c r="D530" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O530" t="inlineStr">
         <is>
@@ -34734,7 +34734,7 @@
         </is>
       </c>
       <c r="D531" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O531" t="inlineStr">
         <is>
@@ -34759,7 +34759,7 @@
         </is>
       </c>
       <c r="D532" s="3" t="n">
-        <v>45834</v>
+        <v>45835</v>
       </c>
       <c r="O532" t="inlineStr">
         <is>

</xml_diff>